<commit_message>
added experiment results anti-copycat
</commit_message>
<xml_diff>
--- a/examples/ipv6/suppression-attack/Mobile-Replay-Defense/CSC_files/Test_csc/random_seed_list.xlsx
+++ b/examples/ipv6/suppression-attack/Mobile-Replay-Defense/CSC_files/Test_csc/random_seed_list.xlsx
@@ -121,16 +121,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,7 +230,11 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -247,21 +247,21 @@
       <c r="A1" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D1" s="2" t="n">
+      <c r="D1" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="2" t="n">
         <v>765765</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="3" t="n">
         <v>487575</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>467854</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="2" t="n">
         <v>293847</v>
       </c>
     </row>
@@ -269,13 +269,13 @@
       <c r="A3" s="0" t="n">
         <v>427044</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="4" t="n">
         <v>427044</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>495363</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="2" t="n">
         <v>876976</v>
       </c>
     </row>
@@ -283,21 +283,21 @@
       <c r="A4" s="1" t="n">
         <v>495363</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>124856</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>124897</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="4" t="n">
         <v>691856</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>124897</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="2" t="n">
         <v>111685</v>
       </c>
     </row>
@@ -308,7 +308,7 @@
       <c r="D6" s="1" t="n">
         <v>169859</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="2" t="n">
         <v>549849</v>
       </c>
     </row>
@@ -319,7 +319,7 @@
       <c r="D7" s="1" t="n">
         <v>154258</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <v>686986</v>
       </c>
     </row>
@@ -330,7 +330,7 @@
       <c r="D8" s="1" t="n">
         <v>155458</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="2" t="n">
         <v>979845</v>
       </c>
     </row>
@@ -341,7 +341,7 @@
       <c r="D9" s="1" t="n">
         <v>124785</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="2" t="n">
         <v>916619</v>
       </c>
     </row>
@@ -352,7 +352,7 @@
       <c r="D10" s="1" t="n">
         <v>125484</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="2" t="n">
         <v>398097</v>
       </c>
     </row>
@@ -379,13 +379,13 @@
       <c r="H13" s="1" t="n">
         <v>111685</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>940022</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="6" t="n">
         <v>963284</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Experiments of ANTICOPYCAT COMPLETED
</commit_message>
<xml_diff>
--- a/examples/ipv6/suppression-attack/Mobile-Replay-Defense/CSC_files/Test_csc/random_seed_list.xlsx
+++ b/examples/ipv6/suppression-attack/Mobile-Replay-Defense/CSC_files/Test_csc/random_seed_list.xlsx
@@ -24,12 +24,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="18">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -47,26 +46,143 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCE181E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC2E0AE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -77,7 +193,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC2E0AE"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -87,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -95,8 +211,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -120,25 +251,76 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,33 +328,50 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC2E0AE"/>
@@ -184,7 +383,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -200,7 +399,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -213,7 +412,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -230,11 +429,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>